<commit_message>
Fixed errors on output sheets.
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_no-graph_output.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_no-graph_output.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="25605" windowHeight="16005" tabRatio="644" firstSheet="13" activeTab="14"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="25605" windowHeight="16005" tabRatio="644" firstSheet="12" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="39">
   <si>
     <t>CIN5</t>
   </si>
@@ -45,9 +45,6 @@
     <t>kk_max</t>
   </si>
   <si>
-    <t>rows genes affected/cols genes controlling</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
   </si>
   <si>
     <t>dcin5</t>
-  </si>
-  <si>
-    <t>prorate</t>
   </si>
   <si>
     <t>Parameter</t>
@@ -665,10 +659,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -676,7 +670,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0.5</v>
@@ -685,7 +679,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -822,7 +816,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -890,7 +884,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -958,7 +952,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1177,7 +1171,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1">
         <v>0.4</v>
@@ -1194,7 +1188,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>6.7986997775525911E-17</v>
@@ -1211,7 +1205,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>3.3993498887762956E-17</v>
@@ -1277,7 +1271,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1">
         <v>0.4</v>
@@ -1294,7 +1288,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>6.7986997775525911E-17</v>
@@ -1311,7 +1305,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>3.3993498887762956E-17</v>
@@ -1370,22 +1364,22 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0.69740719366499726</v>
@@ -1393,7 +1387,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>1.1568003225019745</v>
@@ -1424,19 +1418,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1447,7 +1441,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1.1390375115164613</v>
@@ -1464,7 +1458,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1522,7 +1516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
@@ -1530,15 +1524,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>5.6205951121146291E-3</v>
@@ -1546,7 +1540,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>2.1248299830536412</v>
@@ -1554,7 +1548,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>1.2133358649639586E-33</v>
@@ -1562,7 +1556,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>1012</v>
@@ -1570,23 +1564,23 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
         <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>8.9376526217303694E-3</v>
@@ -1597,7 +1591,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>5.5824917406711817E-3</v>
@@ -1650,15 +1644,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1666,7 +1660,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -1776,7 +1770,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="10">
         <v>0.4</v>
@@ -1818,7 +1812,7 @@
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="10">
         <v>-0.37633430629205178</v>
@@ -1859,7 +1853,7 @@
     </row>
     <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="10">
         <v>-0.22771865423983556</v>
@@ -2028,7 +2022,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="9">
         <v>0.4</v>
@@ -2070,7 +2064,7 @@
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="9">
         <v>-0.37633430629205178</v>
@@ -2111,7 +2105,7 @@
     </row>
     <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="9">
         <v>-0.22771865423983556</v>
@@ -2317,13 +2311,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>0</v>
@@ -2334,7 +2328,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -2351,7 +2345,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -2437,13 +2431,13 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2471,7 +2465,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -2488,7 +2482,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -2560,22 +2554,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2596,7 +2590,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>1000000</v>
@@ -2604,7 +2598,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>1.0000000000000001E-5</v>
@@ -2612,7 +2606,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>1000000</v>
@@ -2620,7 +2614,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>1.0000000000000001E-5</v>
@@ -2628,7 +2622,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -2636,7 +2630,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="8">
         <v>1</v>
@@ -2644,7 +2638,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="8">
         <v>0</v>
@@ -2652,7 +2646,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="8">
         <v>0</v>
@@ -2660,7 +2654,7 @@
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="8">
         <v>0</v>
@@ -2668,7 +2662,7 @@
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" s="8">
         <v>0.4</v>
@@ -2685,18 +2679,18 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="7">
         <v>3</v>
@@ -2707,7 +2701,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="7">
         <v>0</v>
@@ -2718,7 +2712,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2804,15 +2798,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2820,7 +2814,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2866,7 +2860,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -2934,7 +2928,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3002,7 +2996,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>

</xml_diff>